<commit_message>
Removed some extra pads from the CPL file
It was giving a warning inside jlcpcb because some extra pads were in the CPL file
</commit_message>
<xml_diff>
--- a/JLCSMT_CPL1.xlsx
+++ b/JLCSMT_CPL1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My work web\Power Wall\Product Design\PCB Design\Source\MosfetPatch\MosfetPatch_V1\Project Outputs for MosfetPatch_V1\JLCPCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My work web\Power Wall\Documentation\Patch\megacell_mospatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C80A4FD-C5F7-4F16-A626-0C0301787EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A11597-5D48-4391-B7F4-4DFC718CB08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>Designator</t>
   </si>
@@ -43,9 +43,6 @@
     <t>R2</t>
   </si>
   <si>
-    <t>3.3V</t>
-  </si>
-  <si>
     <t>U8</t>
   </si>
   <si>
@@ -119,108 +116,6 @@
   </si>
   <si>
     <t>R1</t>
-  </si>
-  <si>
-    <t>GND</t>
-  </si>
-  <si>
-    <t>C16_G</t>
-  </si>
-  <si>
-    <t>C16+</t>
-  </si>
-  <si>
-    <t>C15_G</t>
-  </si>
-  <si>
-    <t>C15+</t>
-  </si>
-  <si>
-    <t>C14_G</t>
-  </si>
-  <si>
-    <t>C14+</t>
-  </si>
-  <si>
-    <t>C13_G</t>
-  </si>
-  <si>
-    <t>C13+</t>
-  </si>
-  <si>
-    <t>C12_G</t>
-  </si>
-  <si>
-    <t>C12+</t>
-  </si>
-  <si>
-    <t>C11_G</t>
-  </si>
-  <si>
-    <t>C11+</t>
-  </si>
-  <si>
-    <t>C10_G</t>
-  </si>
-  <si>
-    <t>C10+</t>
-  </si>
-  <si>
-    <t>C9_G</t>
-  </si>
-  <si>
-    <t>C9+</t>
-  </si>
-  <si>
-    <t>C8_G</t>
-  </si>
-  <si>
-    <t>C8+</t>
-  </si>
-  <si>
-    <t>C7_G</t>
-  </si>
-  <si>
-    <t>C7+</t>
-  </si>
-  <si>
-    <t>C6_G</t>
-  </si>
-  <si>
-    <t>C6+</t>
-  </si>
-  <si>
-    <t>C5_G</t>
-  </si>
-  <si>
-    <t>C5+</t>
-  </si>
-  <si>
-    <t>C4_G</t>
-  </si>
-  <si>
-    <t>C4+</t>
-  </si>
-  <si>
-    <t>C3_G</t>
-  </si>
-  <si>
-    <t>C3+</t>
-  </si>
-  <si>
-    <t>C2_G</t>
-  </si>
-  <si>
-    <t>C2+</t>
-  </si>
-  <si>
-    <t>C1_G</t>
-  </si>
-  <si>
-    <t>C1+</t>
-  </si>
-  <si>
-    <t>5V</t>
   </si>
 </sst>
 </file>
@@ -569,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -606,10 +501,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="2">
-        <v>207.137</v>
+        <v>37.972999999999999</v>
       </c>
       <c r="C2" s="2">
-        <v>53.975000000000001</v>
+        <v>49.404000000000003</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -623,7 +518,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="2">
-        <v>37.972999999999999</v>
+        <v>88.646000000000001</v>
       </c>
       <c r="C3" s="2">
         <v>49.404000000000003</v>
@@ -640,7 +535,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="2">
-        <v>88.646000000000001</v>
+        <v>139.31899999999999</v>
       </c>
       <c r="C4" s="2">
         <v>49.404000000000003</v>
@@ -657,7 +552,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="2">
-        <v>139.31899999999999</v>
+        <v>189.99199999999999</v>
       </c>
       <c r="C5" s="2">
         <v>49.404000000000003</v>
@@ -674,10 +569,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="2">
-        <v>189.99199999999999</v>
+        <v>228.6</v>
       </c>
       <c r="C6" s="2">
-        <v>49.404000000000003</v>
+        <v>49.402999999999999</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
@@ -691,7 +586,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2">
-        <v>228.6</v>
+        <v>276.94470000000001</v>
       </c>
       <c r="C7" s="2">
         <v>49.402999999999999</v>
@@ -708,7 +603,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="2">
-        <v>276.94470000000001</v>
+        <v>325.28930000000003</v>
       </c>
       <c r="C8" s="2">
         <v>49.402999999999999</v>
@@ -725,7 +620,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="2">
-        <v>325.28930000000003</v>
+        <v>373.63400000000001</v>
       </c>
       <c r="C9" s="2">
         <v>49.402999999999999</v>
@@ -742,16 +637,16 @@
         <v>15</v>
       </c>
       <c r="B10" s="2">
-        <v>373.63400000000001</v>
+        <v>30.988</v>
       </c>
       <c r="C10" s="2">
-        <v>49.402999999999999</v>
+        <v>49.656999999999996</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -759,7 +654,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="2">
-        <v>30.988</v>
+        <v>44.831000000000003</v>
       </c>
       <c r="C11" s="2">
         <v>49.656999999999996</v>
@@ -768,7 +663,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -776,7 +671,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="2">
-        <v>44.831000000000003</v>
+        <v>80.518000000000001</v>
       </c>
       <c r="C12" s="2">
         <v>49.656999999999996</v>
@@ -785,7 +680,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="2">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -793,7 +688,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="2">
-        <v>80.518000000000001</v>
+        <v>94.742000000000004</v>
       </c>
       <c r="C13" s="2">
         <v>49.656999999999996</v>
@@ -802,7 +697,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -810,7 +705,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="2">
-        <v>94.742000000000004</v>
+        <v>132.08000000000001</v>
       </c>
       <c r="C14" s="2">
         <v>49.656999999999996</v>
@@ -819,7 +714,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="2">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -827,7 +722,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="2">
-        <v>132.08000000000001</v>
+        <v>146.17699999999999</v>
       </c>
       <c r="C15" s="2">
         <v>49.656999999999996</v>
@@ -836,7 +731,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -844,7 +739,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="2">
-        <v>146.17699999999999</v>
+        <v>180.59399999999999</v>
       </c>
       <c r="C16" s="2">
         <v>49.656999999999996</v>
@@ -853,7 +748,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="2">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -861,7 +756,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="2">
-        <v>180.59399999999999</v>
+        <v>196.46899999999999</v>
       </c>
       <c r="C17" s="2">
         <v>49.656999999999996</v>
@@ -870,7 +765,7 @@
         <v>5</v>
       </c>
       <c r="E17" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -878,7 +773,7 @@
         <v>23</v>
       </c>
       <c r="B18" s="2">
-        <v>196.46899999999999</v>
+        <v>221.74199999999999</v>
       </c>
       <c r="C18" s="2">
         <v>49.656999999999996</v>
@@ -887,7 +782,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="2">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -895,7 +790,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="2">
-        <v>221.74199999999999</v>
+        <v>235.7987</v>
       </c>
       <c r="C19" s="2">
         <v>49.656999999999996</v>
@@ -904,7 +799,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -912,7 +807,7 @@
         <v>25</v>
       </c>
       <c r="B20" s="2">
-        <v>235.7987</v>
+        <v>267.75630000000001</v>
       </c>
       <c r="C20" s="2">
         <v>49.656999999999996</v>
@@ -921,7 +816,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="2">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -929,7 +824,7 @@
         <v>26</v>
       </c>
       <c r="B21" s="2">
-        <v>267.75630000000001</v>
+        <v>283.59100000000001</v>
       </c>
       <c r="C21" s="2">
         <v>49.656999999999996</v>
@@ -938,7 +833,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -946,7 +841,7 @@
         <v>27</v>
       </c>
       <c r="B22" s="2">
-        <v>283.59100000000001</v>
+        <v>317.88099999999997</v>
       </c>
       <c r="C22" s="2">
         <v>49.656999999999996</v>
@@ -955,7 +850,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="2">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -963,7 +858,7 @@
         <v>28</v>
       </c>
       <c r="B23" s="2">
-        <v>317.88099999999997</v>
+        <v>332.23200000000003</v>
       </c>
       <c r="C23" s="2">
         <v>49.656999999999996</v>
@@ -972,7 +867,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -980,7 +875,7 @@
         <v>29</v>
       </c>
       <c r="B24" s="2">
-        <v>332.23200000000003</v>
+        <v>365.887</v>
       </c>
       <c r="C24" s="2">
         <v>49.656999999999996</v>
@@ -989,7 +884,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="2">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -997,7 +892,7 @@
         <v>30</v>
       </c>
       <c r="B25" s="2">
-        <v>365.887</v>
+        <v>380.61900000000003</v>
       </c>
       <c r="C25" s="2">
         <v>49.656999999999996</v>
@@ -1006,637 +901,280 @@
         <v>5</v>
       </c>
       <c r="E25" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B26" s="2">
-        <v>380.61900000000003</v>
+        <v>204.851</v>
       </c>
       <c r="C26" s="2">
-        <v>49.656999999999996</v>
+        <v>47.625</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="2">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B27" s="2">
-        <v>204.851</v>
+        <v>206.88300000000001</v>
       </c>
       <c r="C27" s="2">
-        <v>47.625</v>
+        <v>48.640999999999998</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="2">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="2">
-        <v>206.88300000000001</v>
-      </c>
-      <c r="C28" s="2">
-        <v>48.640999999999998</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="2">
-        <v>180</v>
-      </c>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="2">
-        <v>210.947</v>
-      </c>
-      <c r="C29" s="2">
-        <v>53.975000000000001</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="2">
-        <v>90</v>
-      </c>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="2">
-        <v>31.242000000000001</v>
-      </c>
-      <c r="C30" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="2">
-        <v>90</v>
-      </c>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="2">
-        <v>31.242000000000001</v>
-      </c>
-      <c r="C31" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="2">
-        <v>90</v>
-      </c>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="2">
-        <v>43.814999999999998</v>
-      </c>
-      <c r="C32" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="2">
-        <v>90</v>
-      </c>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="2">
-        <v>43.814999999999998</v>
-      </c>
-      <c r="C33" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="2">
-        <v>90</v>
-      </c>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="2">
-        <v>81.787999999999997</v>
-      </c>
-      <c r="C34" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="2">
-        <v>90</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" s="2">
-        <v>81.787999999999997</v>
-      </c>
-      <c r="C35" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="2">
-        <v>90</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" s="2">
-        <v>94.614999999999995</v>
-      </c>
-      <c r="C36" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="2">
-        <v>90</v>
-      </c>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" s="2">
-        <v>94.614999999999995</v>
-      </c>
-      <c r="C37" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="2">
-        <v>90</v>
-      </c>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="2">
-        <v>132.334</v>
-      </c>
-      <c r="C38" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="2">
-        <v>90</v>
-      </c>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="2">
-        <v>132.334</v>
-      </c>
-      <c r="C39" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="2">
-        <v>90</v>
-      </c>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="2">
-        <v>145.66900000000001</v>
-      </c>
-      <c r="C40" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" s="2">
-        <v>90</v>
-      </c>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="2">
-        <v>145.66900000000001</v>
-      </c>
-      <c r="C41" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="2">
-        <v>90</v>
-      </c>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="2">
-        <v>182.75299999999999</v>
-      </c>
-      <c r="C42" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="2">
-        <v>90</v>
-      </c>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="2">
-        <v>182.75299999999999</v>
-      </c>
-      <c r="C43" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" s="2">
-        <v>90</v>
-      </c>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="2">
-        <v>195.072</v>
-      </c>
-      <c r="C44" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" s="2">
-        <v>90</v>
-      </c>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="2">
-        <v>195.072</v>
-      </c>
-      <c r="C45" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" s="2">
-        <v>90</v>
-      </c>
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="2">
-        <v>223.13900000000001</v>
-      </c>
-      <c r="C46" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" s="2">
-        <v>90</v>
-      </c>
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="2">
-        <v>223.13900000000001</v>
-      </c>
-      <c r="C47" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" s="2">
-        <v>90</v>
-      </c>
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" s="2">
-        <v>235.58500000000001</v>
-      </c>
-      <c r="C48" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="2">
-        <v>90</v>
-      </c>
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B49" s="2">
-        <v>235.58500000000001</v>
-      </c>
-      <c r="C49" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" s="2">
-        <v>90</v>
-      </c>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50" s="2">
-        <v>268.60500000000002</v>
-      </c>
-      <c r="C50" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" s="2">
-        <v>90</v>
-      </c>
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51" s="2">
-        <v>268.60500000000002</v>
-      </c>
-      <c r="C51" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" s="2">
-        <v>90</v>
-      </c>
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="2">
-        <v>283.59100000000001</v>
-      </c>
-      <c r="C52" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E52" s="2">
-        <v>90</v>
-      </c>
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B53" s="2">
-        <v>283.59100000000001</v>
-      </c>
-      <c r="C53" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E53" s="2">
-        <v>90</v>
-      </c>
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54" s="2">
-        <v>318.51600000000002</v>
-      </c>
-      <c r="C54" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E54" s="2">
-        <v>90</v>
-      </c>
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B55" s="2">
-        <v>318.51600000000002</v>
-      </c>
-      <c r="C55" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E55" s="2">
-        <v>90</v>
-      </c>
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" s="2">
-        <v>331.59699999999998</v>
-      </c>
-      <c r="C56" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E56" s="2">
-        <v>90</v>
-      </c>
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B57" s="2">
-        <v>331.59699999999998</v>
-      </c>
-      <c r="C57" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E57" s="2">
-        <v>90</v>
-      </c>
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B58" s="2">
-        <v>366.52199999999999</v>
-      </c>
-      <c r="C58" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E58" s="2">
-        <v>90</v>
-      </c>
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B59" s="2">
-        <v>366.52199999999999</v>
-      </c>
-      <c r="C59" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" s="2">
-        <v>90</v>
-      </c>
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B60" s="2">
-        <v>379.98399999999998</v>
-      </c>
-      <c r="C60" s="2">
-        <v>45.847000000000001</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E60" s="2">
-        <v>90</v>
-      </c>
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B61" s="2">
-        <v>379.98399999999998</v>
-      </c>
-      <c r="C61" s="2">
-        <v>54.228999999999999</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E61" s="2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B62" s="2">
-        <v>214.75700000000001</v>
-      </c>
-      <c r="C62" s="2">
-        <v>53.975000000000001</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E62" s="2">
-        <v>90</v>
-      </c>
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>